<commit_message>
Functional Testing Assignments Completed
</commit_message>
<xml_diff>
--- a/Training/GoogleKeep_Monira.xlsx
+++ b/Training/GoogleKeep_Monira.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Documents\GitDemo\SQAT\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF096C69-03C6-4EA2-98CF-42BC57A2FAC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE01F8B-FC52-49A0-841B-709735A7A305}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -770,7 +770,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
       <c r="J4" s="26"/>
       <c r="K4" s="26"/>
     </row>
-    <row r="5" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>2</v>
       </c>

</xml_diff>